<commit_message>
seminar tesisi 2 data sisa
</commit_message>
<xml_diff>
--- a/tabel hasil prediksi segmentasi.xlsx
+++ b/tabel hasil prediksi segmentasi.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="62">
   <si>
     <t>No</t>
   </si>
@@ -389,9 +389,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -407,6 +404,11 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -428,11 +430,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,11 +471,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -485,13 +485,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Pengujian</a:t>
+              <a:t>Pengujian Segmentasi</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Segmentasi</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -508,11 +503,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -547,17 +542,10 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:alpha val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:alpha val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -571,15 +559,18 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -589,7 +580,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -604,9 +595,9 @@
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
                     </a:ln>
@@ -661,17 +652,10 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:alpha val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:alpha val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -685,15 +669,18 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -703,7 +690,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -718,9 +705,9 @@
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
                     </a:ln>
@@ -775,17 +762,10 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:alpha val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:alpha val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -799,15 +779,18 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -817,7 +800,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -832,9 +815,9 @@
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
                     </a:ln>
@@ -874,7 +857,7 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="inEnd"/>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -882,7 +865,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="65"/>
+        <c:gapWidth val="444"/>
+        <c:overlap val="-90"/>
         <c:axId val="795141663"/>
         <c:axId val="785369279"/>
       </c:barChart>
@@ -893,17 +877,31 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -915,11 +913,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -944,32 +942,6 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="95000"/>
-                      <a:lumOff val="5000"/>
-                      <a:alpha val="42000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                      <a:alpha val="36000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -987,15 +959,10 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="39000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1008,9 +975,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1027,30 +994,14 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="39000">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="lt1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="25000"/>
-          <a:lumOff val="75000"/>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -1116,43 +1067,43 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="205">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
-  <cs:chartArea>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1160,30 +1111,14 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-          <a:gs pos="39000">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1196,27 +1131,40 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-          <a:alpha val="75000"/>
-        </a:schemeClr>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
@@ -1232,18 +1180,8 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -1257,18 +1195,8 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -1281,18 +1209,18 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="31750" cap="rnd">
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="85000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
@@ -1302,13 +1230,17 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -1332,17 +1264,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1359,15 +1291,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1383,12 +1315,11 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1402,7 +1333,7 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -1428,24 +1359,12 @@
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-                <a:alpha val="42000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="75000"/>
-                <a:alpha val="36000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -1459,24 +1378,12 @@
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-                <a:alpha val="42000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="75000"/>
-                <a:alpha val="36000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1490,12 +1397,11 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1509,9 +1415,9 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1522,22 +1428,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="95000"/>
-          <a:alpha val="39000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1545,7 +1443,7 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1558,17 +1456,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1586,9 +1484,9 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1600,12 +1498,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1621,6 +1519,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1629,12 +1528,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -1649,7 +1548,7 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -1662,14 +1561,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
-        <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2023,10 +1928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K103"/>
+  <dimension ref="A1:K127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="G109" sqref="G109"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="G121" sqref="G121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,24 +1950,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -2341,24 +2246,24 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
@@ -2600,24 +2505,24 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
@@ -3049,246 +2954,246 @@
       </c>
     </row>
     <row r="54" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B54" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="15" t="s">
+      <c r="B54" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D54" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E54" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F54" s="10" t="s">
+      <c r="F54" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G54" s="17" t="s">
+      <c r="G54" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="11" t="s">
+      <c r="B55" s="18"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="F55" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G55" s="18"/>
+      <c r="G55" s="20"/>
     </row>
     <row r="56" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="12">
+      <c r="B56" s="11">
         <v>1</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C56" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D56" s="11">
+      <c r="D56" s="10">
         <v>24</v>
       </c>
-      <c r="E56" s="11">
+      <c r="E56" s="10">
         <v>22</v>
       </c>
-      <c r="F56" s="11">
+      <c r="F56" s="10">
         <v>4</v>
       </c>
-      <c r="G56" s="14">
+      <c r="G56" s="13">
         <v>0.83</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="12">
+      <c r="B57" s="11">
         <v>2</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C57" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D57" s="11">
+      <c r="D57" s="10">
         <v>17</v>
       </c>
-      <c r="E57" s="11">
+      <c r="E57" s="10">
         <v>17</v>
       </c>
-      <c r="F57" s="11">
-        <v>0</v>
-      </c>
-      <c r="G57" s="14">
+      <c r="F57" s="10">
+        <v>0</v>
+      </c>
+      <c r="G57" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="12">
+      <c r="B58" s="11">
         <v>3</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C58" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D58" s="11">
+      <c r="D58" s="10">
         <v>21</v>
       </c>
-      <c r="E58" s="11">
+      <c r="E58" s="10">
         <v>21</v>
       </c>
-      <c r="F58" s="11">
+      <c r="F58" s="10">
         <v>2</v>
       </c>
-      <c r="G58" s="14">
+      <c r="G58" s="13">
         <v>0.9</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="12">
+      <c r="B59" s="11">
         <v>4</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D59" s="11">
+      <c r="D59" s="10">
         <v>17</v>
       </c>
-      <c r="E59" s="11">
+      <c r="E59" s="10">
         <v>15</v>
       </c>
-      <c r="F59" s="11">
+      <c r="F59" s="10">
         <v>2</v>
       </c>
-      <c r="G59" s="14">
+      <c r="G59" s="13">
         <v>0.88</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="12">
+      <c r="B60" s="11">
         <v>5</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C60" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D60" s="11">
+      <c r="D60" s="10">
         <v>13</v>
       </c>
-      <c r="E60" s="11">
+      <c r="E60" s="10">
         <v>13</v>
       </c>
-      <c r="F60" s="11">
-        <v>0</v>
-      </c>
-      <c r="G60" s="14">
+      <c r="F60" s="10">
+        <v>0</v>
+      </c>
+      <c r="G60" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="12">
+      <c r="B61" s="11">
         <v>6</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C61" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D61" s="11">
+      <c r="D61" s="10">
         <v>21</v>
       </c>
-      <c r="E61" s="11">
+      <c r="E61" s="10">
         <v>17</v>
       </c>
-      <c r="F61" s="11">
+      <c r="F61" s="10">
         <v>4</v>
       </c>
-      <c r="G61" s="14">
+      <c r="G61" s="13">
         <v>0.8</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="12">
+      <c r="B62" s="11">
         <v>7</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C62" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D62" s="11">
+      <c r="D62" s="10">
         <v>14</v>
       </c>
-      <c r="E62" s="11">
+      <c r="E62" s="10">
         <v>10</v>
       </c>
-      <c r="F62" s="11">
+      <c r="F62" s="10">
         <v>4</v>
       </c>
-      <c r="G62" s="14">
+      <c r="G62" s="13">
         <v>0.71</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="12">
+      <c r="B63" s="11">
         <v>8</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C63" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D63" s="11">
+      <c r="D63" s="10">
         <v>14</v>
       </c>
-      <c r="E63" s="11">
+      <c r="E63" s="10">
         <v>14</v>
       </c>
-      <c r="F63" s="11">
-        <v>0</v>
-      </c>
-      <c r="G63" s="14">
+      <c r="F63" s="10">
+        <v>0</v>
+      </c>
+      <c r="G63" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="12">
+      <c r="B64" s="11">
         <v>9</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="C64" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D64" s="11">
+      <c r="D64" s="10">
         <v>18</v>
       </c>
-      <c r="E64" s="11">
+      <c r="E64" s="10">
         <v>14</v>
       </c>
-      <c r="F64" s="11">
+      <c r="F64" s="10">
         <v>4</v>
       </c>
-      <c r="G64" s="14">
+      <c r="G64" s="13">
         <v>0.77</v>
       </c>
     </row>
     <row r="65" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="12">
+      <c r="B65" s="11">
         <v>10</v>
       </c>
-      <c r="C65" s="13" t="s">
+      <c r="C65" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D65" s="11">
+      <c r="D65" s="10">
         <v>21</v>
       </c>
-      <c r="E65" s="11">
+      <c r="E65" s="10">
         <v>19</v>
       </c>
-      <c r="F65" s="11">
+      <c r="F65" s="10">
         <v>2</v>
       </c>
-      <c r="G65" s="14">
+      <c r="G65" s="13">
         <v>0.9</v>
       </c>
     </row>
     <row r="66" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="19" t="s">
+      <c r="B66" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C66" s="20"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="14">
+      <c r="C66" s="22"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="13">
         <f>SUM(G56:G65)/10</f>
         <v>0.87899999999999989</v>
       </c>
@@ -3299,244 +3204,244 @@
       </c>
     </row>
     <row r="69" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B69" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C69" s="15" t="s">
+      <c r="B69" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D69" s="17" t="s">
+      <c r="D69" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E69" s="10" t="s">
+      <c r="E69" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F69" s="10" t="s">
+      <c r="F69" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="17" t="s">
+      <c r="G69" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="70" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="11" t="s">
+      <c r="B70" s="18"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F70" s="11" t="s">
+      <c r="F70" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G70" s="18"/>
+      <c r="G70" s="20"/>
     </row>
     <row r="71" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="12">
+      <c r="B71" s="11">
         <v>1</v>
       </c>
-      <c r="C71" s="13" t="s">
+      <c r="C71" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D71" s="11">
+      <c r="D71" s="10">
         <v>24</v>
       </c>
-      <c r="E71" s="11">
+      <c r="E71" s="10">
         <v>22</v>
       </c>
-      <c r="F71" s="11">
+      <c r="F71" s="10">
         <v>2</v>
       </c>
-      <c r="G71" s="14">
+      <c r="G71" s="13">
         <v>0.91</v>
       </c>
     </row>
     <row r="72" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="12">
+      <c r="B72" s="11">
         <v>2</v>
       </c>
-      <c r="C72" s="13" t="s">
+      <c r="C72" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D72" s="11">
+      <c r="D72" s="10">
         <v>17</v>
       </c>
-      <c r="E72" s="11">
+      <c r="E72" s="10">
         <v>17</v>
       </c>
-      <c r="F72" s="11">
-        <v>0</v>
-      </c>
-      <c r="G72" s="14">
+      <c r="F72" s="10">
+        <v>0</v>
+      </c>
+      <c r="G72" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="12">
+      <c r="B73" s="11">
         <v>3</v>
       </c>
-      <c r="C73" s="13" t="s">
+      <c r="C73" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D73" s="11">
+      <c r="D73" s="10">
         <v>21</v>
       </c>
-      <c r="E73" s="11">
+      <c r="E73" s="10">
         <v>21</v>
       </c>
-      <c r="F73" s="11">
+      <c r="F73" s="10">
         <v>1</v>
       </c>
-      <c r="G73" s="14">
+      <c r="G73" s="13">
         <v>0.95</v>
       </c>
     </row>
     <row r="74" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="12">
+      <c r="B74" s="11">
         <v>4</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="C74" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D74" s="11">
+      <c r="D74" s="10">
         <v>17</v>
       </c>
-      <c r="E74" s="11">
+      <c r="E74" s="10">
         <v>17</v>
       </c>
-      <c r="F74" s="11">
-        <v>0</v>
-      </c>
-      <c r="G74" s="14">
+      <c r="F74" s="10">
+        <v>0</v>
+      </c>
+      <c r="G74" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="12">
+      <c r="B75" s="11">
         <v>5</v>
       </c>
-      <c r="C75" s="13" t="s">
+      <c r="C75" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D75" s="11">
+      <c r="D75" s="10">
         <v>13</v>
       </c>
-      <c r="E75" s="11">
+      <c r="E75" s="10">
         <v>11</v>
       </c>
-      <c r="F75" s="11">
+      <c r="F75" s="10">
         <v>2</v>
       </c>
-      <c r="G75" s="14">
+      <c r="G75" s="13">
         <v>0.84</v>
       </c>
     </row>
     <row r="76" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="12">
+      <c r="B76" s="11">
         <v>6</v>
       </c>
-      <c r="C76" s="13" t="s">
+      <c r="C76" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D76" s="11">
+      <c r="D76" s="10">
         <v>21</v>
       </c>
-      <c r="E76" s="11">
+      <c r="E76" s="10">
         <v>20</v>
       </c>
-      <c r="F76" s="11">
+      <c r="F76" s="10">
         <v>1</v>
       </c>
-      <c r="G76" s="14">
+      <c r="G76" s="13">
         <v>0.95</v>
       </c>
     </row>
     <row r="77" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="12">
+      <c r="B77" s="11">
         <v>7</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C77" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D77" s="11">
+      <c r="D77" s="10">
         <v>14</v>
       </c>
-      <c r="E77" s="11">
+      <c r="E77" s="10">
         <v>13</v>
       </c>
-      <c r="F77" s="11">
+      <c r="F77" s="10">
         <v>1</v>
       </c>
-      <c r="G77" s="14">
+      <c r="G77" s="13">
         <v>0.92</v>
       </c>
     </row>
     <row r="78" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="12">
+      <c r="B78" s="11">
         <v>8</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="C78" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D78" s="11">
+      <c r="D78" s="10">
         <v>14</v>
       </c>
-      <c r="E78" s="11">
+      <c r="E78" s="10">
         <v>14</v>
       </c>
-      <c r="F78" s="11">
-        <v>0</v>
-      </c>
-      <c r="G78" s="14">
+      <c r="F78" s="10">
+        <v>0</v>
+      </c>
+      <c r="G78" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="12">
+      <c r="B79" s="11">
         <v>9</v>
       </c>
-      <c r="C79" s="13" t="s">
+      <c r="C79" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D79" s="11">
+      <c r="D79" s="10">
         <v>18</v>
       </c>
-      <c r="E79" s="11">
+      <c r="E79" s="10">
         <v>18</v>
       </c>
-      <c r="F79" s="11">
-        <v>0</v>
-      </c>
-      <c r="G79" s="14">
+      <c r="F79" s="10">
+        <v>0</v>
+      </c>
+      <c r="G79" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="12">
+      <c r="B80" s="11">
         <v>10</v>
       </c>
-      <c r="C80" s="13" t="s">
+      <c r="C80" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D80" s="11">
+      <c r="D80" s="10">
         <v>21</v>
       </c>
-      <c r="E80" s="11">
+      <c r="E80" s="10">
         <v>20</v>
       </c>
-      <c r="F80" s="11">
+      <c r="F80" s="10">
         <v>1</v>
       </c>
-      <c r="G80" s="14">
+      <c r="G80" s="13">
         <v>0.95</v>
       </c>
     </row>
     <row r="81" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="12"/>
-      <c r="C81" s="13"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="14">
+      <c r="B81" s="11"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+      <c r="G81" s="13">
         <f>SUM(G71:G80)/10</f>
         <v>0.95199999999999996</v>
       </c>
@@ -3547,282 +3452,325 @@
       </c>
     </row>
     <row r="84" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B84" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C84" s="15" t="s">
+      <c r="B84" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D84" s="17" t="s">
+      <c r="D84" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E84" s="10" t="s">
+      <c r="E84" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F84" s="10" t="s">
+      <c r="F84" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G84" s="17" t="s">
+      <c r="G84" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="85" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="16"/>
-      <c r="C85" s="16"/>
-      <c r="D85" s="18"/>
-      <c r="E85" s="11" t="s">
+      <c r="B85" s="18"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="20"/>
+      <c r="E85" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F85" s="11" t="s">
+      <c r="F85" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G85" s="18"/>
+      <c r="G85" s="20"/>
     </row>
     <row r="86" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="12">
+      <c r="B86" s="11">
         <v>1</v>
       </c>
-      <c r="C86" s="13" t="s">
+      <c r="C86" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D86" s="11">
+      <c r="D86" s="10">
         <v>24</v>
       </c>
-      <c r="E86" s="11">
+      <c r="E86" s="10">
         <v>24</v>
       </c>
-      <c r="F86" s="11">
-        <v>0</v>
-      </c>
-      <c r="G86" s="14">
+      <c r="F86" s="10">
+        <v>0</v>
+      </c>
+      <c r="G86" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="12">
+      <c r="B87" s="11">
         <v>2</v>
       </c>
-      <c r="C87" s="13" t="s">
+      <c r="C87" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D87" s="11">
+      <c r="D87" s="10">
         <v>17</v>
       </c>
-      <c r="E87" s="11">
+      <c r="E87" s="10">
         <v>17</v>
       </c>
-      <c r="F87" s="11">
-        <v>0</v>
-      </c>
-      <c r="G87" s="14">
+      <c r="F87" s="10">
+        <v>0</v>
+      </c>
+      <c r="G87" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="12">
+      <c r="B88" s="11">
         <v>3</v>
       </c>
-      <c r="C88" s="13" t="s">
+      <c r="C88" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D88" s="11">
+      <c r="D88" s="10">
         <v>21</v>
       </c>
-      <c r="E88" s="11">
+      <c r="E88" s="10">
         <v>21</v>
       </c>
-      <c r="F88" s="11">
-        <v>0</v>
-      </c>
-      <c r="G88" s="14">
+      <c r="F88" s="10">
+        <v>0</v>
+      </c>
+      <c r="G88" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="12">
+      <c r="B89" s="11">
         <v>4</v>
       </c>
-      <c r="C89" s="13" t="s">
+      <c r="C89" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D89" s="11">
+      <c r="D89" s="10">
         <v>17</v>
       </c>
-      <c r="E89" s="11">
+      <c r="E89" s="10">
         <v>17</v>
       </c>
-      <c r="F89" s="11">
-        <v>0</v>
-      </c>
-      <c r="G89" s="14">
+      <c r="F89" s="10">
+        <v>0</v>
+      </c>
+      <c r="G89" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="90" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="12">
+      <c r="B90" s="11">
         <v>5</v>
       </c>
-      <c r="C90" s="13" t="s">
+      <c r="C90" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D90" s="11">
+      <c r="D90" s="10">
         <v>13</v>
       </c>
-      <c r="E90" s="11">
+      <c r="E90" s="10">
         <v>13</v>
       </c>
-      <c r="F90" s="11">
-        <v>0</v>
-      </c>
-      <c r="G90" s="14">
+      <c r="F90" s="10">
+        <v>0</v>
+      </c>
+      <c r="G90" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="12">
+      <c r="B91" s="11">
         <v>6</v>
       </c>
-      <c r="C91" s="13" t="s">
+      <c r="C91" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D91" s="11">
+      <c r="D91" s="10">
         <v>21</v>
       </c>
-      <c r="E91" s="11">
+      <c r="E91" s="10">
         <v>19</v>
       </c>
-      <c r="F91" s="11">
+      <c r="F91" s="10">
         <v>2</v>
       </c>
-      <c r="G91" s="14">
+      <c r="G91" s="13">
         <v>0.9</v>
       </c>
     </row>
     <row r="92" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="12">
+      <c r="B92" s="11">
         <v>7</v>
       </c>
-      <c r="C92" s="13" t="s">
+      <c r="C92" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D92" s="11">
+      <c r="D92" s="10">
         <v>14</v>
       </c>
-      <c r="E92" s="11">
+      <c r="E92" s="10">
         <v>14</v>
       </c>
-      <c r="F92" s="11">
-        <v>0</v>
-      </c>
-      <c r="G92" s="14">
+      <c r="F92" s="10">
+        <v>0</v>
+      </c>
+      <c r="G92" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="12">
+      <c r="B93" s="11">
         <v>8</v>
       </c>
-      <c r="C93" s="13" t="s">
+      <c r="C93" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D93" s="11">
+      <c r="D93" s="10">
         <v>14</v>
       </c>
-      <c r="E93" s="11">
+      <c r="E93" s="10">
         <v>14</v>
       </c>
-      <c r="F93" s="11">
-        <v>0</v>
-      </c>
-      <c r="G93" s="14">
+      <c r="F93" s="10">
+        <v>0</v>
+      </c>
+      <c r="G93" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="12">
+      <c r="B94" s="11">
         <v>9</v>
       </c>
-      <c r="C94" s="13" t="s">
+      <c r="C94" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D94" s="11">
+      <c r="D94" s="10">
         <v>18</v>
       </c>
-      <c r="E94" s="11">
+      <c r="E94" s="10">
         <v>18</v>
       </c>
-      <c r="F94" s="11">
-        <v>0</v>
-      </c>
-      <c r="G94" s="14">
+      <c r="F94" s="10">
+        <v>0</v>
+      </c>
+      <c r="G94" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="12">
+      <c r="B95" s="11">
         <v>10</v>
       </c>
-      <c r="C95" s="13" t="s">
+      <c r="C95" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D95" s="11">
+      <c r="D95" s="10">
         <v>21</v>
       </c>
-      <c r="E95" s="11">
+      <c r="E95" s="10">
         <v>19</v>
       </c>
-      <c r="F95" s="11">
+      <c r="F95" s="10">
         <v>2</v>
       </c>
-      <c r="G95" s="14">
+      <c r="G95" s="13">
         <v>0.9</v>
       </c>
     </row>
     <row r="96" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="12"/>
-      <c r="C96" s="13"/>
-      <c r="D96" s="11"/>
-      <c r="E96" s="11"/>
-      <c r="F96" s="11"/>
-      <c r="G96" s="22">
+      <c r="B96" s="11"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="10"/>
+      <c r="E96" s="10"/>
+      <c r="F96" s="10"/>
+      <c r="G96" s="14">
         <f>SUM(G86:G95)/10</f>
         <v>0.98000000000000009</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="23" t="s">
+      <c r="B100" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C100" s="23" t="s">
+      <c r="C100" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B101" s="23" t="s">
+      <c r="B101" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C101" s="24">
+      <c r="C101" s="16">
         <v>0.88</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B102" s="23" t="s">
+      <c r="B102" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C102" s="24">
+      <c r="C102" s="16">
         <v>0.95</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B103" s="23" t="s">
+      <c r="B103" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C103" s="24">
+      <c r="C103" s="16">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B124" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C124" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D124" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E124" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B125" s="15"/>
+      <c r="C125" s="16">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B126" s="15"/>
+      <c r="C126" s="16">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B127" s="15"/>
+      <c r="C127" s="16">
         <v>0.98</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="B66:F66"/>
     <mergeCell ref="B69:B70"/>
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="D69:D70"/>
@@ -3831,17 +3779,6 @@
     <mergeCell ref="C84:C85"/>
     <mergeCell ref="D84:D85"/>
     <mergeCell ref="G84:G85"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A35:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>